<commit_message>
Added info about users
</commit_message>
<xml_diff>
--- a/Ecommerce Data/All queries/Count of purchase in hour.xlsx
+++ b/Ecommerce Data/All queries/Count of purchase in hour.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Analyst Projects\Ecommerce Data\All queries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AAF137-23D8-4DE5-BAD3-E24E701A51E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8E111C-7B4A-441D-B44C-E489EAEA32AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>hour</t>
+    <t>Hour</t>
   </si>
   <si>
-    <t>CountOfProduct</t>
+    <t>Sum Count Of Purchased Products</t>
   </si>
 </sst>
 </file>
@@ -887,7 +887,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>